<commit_message>
script_svm atualizado com sensibilidade e acurácia, modelo poligonal 0,05 restaurado
</commit_message>
<xml_diff>
--- a/Python/54BND_svm.xlsx
+++ b/Python/54BND_svm.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Rodrigo S. Hirama\Documentos\EACH\IC\Classification-of-mammography-images\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDE1864-7A3A-478A-A755-B69FE1A03E3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683D2463-6C13-4E2D-AC56-09EFDA222549}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="0,01" sheetId="1" r:id="rId1"/>
-    <sheet name="0,001" sheetId="2" r:id="rId2"/>
+    <sheet name="54BND" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>rbf</t>
   </si>
@@ -35,13 +34,19 @@
     <t>accuracy</t>
   </si>
   <si>
-    <t>std_dev</t>
+    <t>sensibility</t>
+  </si>
+  <si>
+    <t>specificity</t>
   </si>
   <si>
     <t>0,001</t>
   </si>
   <si>
     <t>0,01</t>
+  </si>
+  <si>
+    <t>0,05</t>
   </si>
 </sst>
 </file>
@@ -447,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,21 +479,35 @@
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -510,8 +529,17 @@
       <c r="G3">
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -533,8 +561,17 @@
       <c r="G4">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -556,8 +593,17 @@
       <c r="G5">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -579,8 +625,17 @@
       <c r="G6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J6">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -602,8 +657,17 @@
       <c r="G7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J7">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -625,8 +689,17 @@
       <c r="G8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I8">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J8">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -648,8 +721,17 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J9">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -671,8 +753,17 @@
       <c r="G10">
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J10">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -694,8 +785,17 @@
       <c r="G11">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I11">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J11">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -717,8 +817,17 @@
       <c r="G12">
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J12">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -740,8 +849,17 @@
       <c r="G13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J13">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -763,8 +881,17 @@
       <c r="G14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I14">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J14">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -786,8 +913,17 @@
       <c r="G15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -809,8 +945,17 @@
       <c r="G16">
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J16">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -832,8 +977,17 @@
       <c r="G17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0.5</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -855,8 +1009,17 @@
       <c r="G18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -878,8 +1041,17 @@
       <c r="G19">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>0.5</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -901,8 +1073,17 @@
       <c r="G20">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -924,8 +1105,17 @@
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -947,70 +1137,118 @@
       <c r="G22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B23">
-        <v>0.73333333333333328</v>
+        <v>0.7407407407407407</v>
       </c>
       <c r="C23">
-        <v>0.65833333333333333</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D23">
-        <v>0.71666666666666656</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="E23">
-        <v>0.75</v>
+        <v>0.7592592592592593</v>
       </c>
       <c r="F23">
-        <v>0.67500000000000004</v>
+        <v>0.68518518518518523</v>
       </c>
       <c r="G23">
-        <v>0.73333333333333328</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="H23">
+        <v>0.42592592592592587</v>
+      </c>
+      <c r="I23">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J23">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B24">
-        <v>0.28577380332470409</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="C24">
-        <v>0.2762597409041796</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="D24">
-        <v>0.27938424357067021</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="E24">
-        <v>0.29107081994288297</v>
+        <v>0.6071428571428571</v>
       </c>
       <c r="F24">
-        <v>0.26601482832520612</v>
+        <v>0.75</v>
       </c>
       <c r="G24">
-        <v>0.30459444804161778</v>
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="H24">
+        <v>0.8214285714285714</v>
+      </c>
+      <c r="I24">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="J24">
+        <v>0.6071428571428571</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="C25">
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="D25">
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="E25">
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="F25">
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="G25">
+        <v>0.88461538461538458</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>3.8461538461538457E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>